<commit_message>
Inclusión de nuevos datos
</commit_message>
<xml_diff>
--- a/data/datos.xlsx
+++ b/data/datos.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RENTERIA" sheetId="4" r:id="rId1"/>
     <sheet name="ECHO" sheetId="3" r:id="rId2"/>
     <sheet name="INE" sheetId="5" r:id="rId3"/>
+    <sheet name="CED" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>anio</t>
   </si>
@@ -439,7 +440,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G4" sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -690,7 +691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -926,4 +927,123 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2006</v>
+      </c>
+      <c r="B2">
+        <f>D2+F2</f>
+        <v>17.700000000000003</v>
+      </c>
+      <c r="C2">
+        <f>E2+G2</f>
+        <v>21.599999999999998</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>12.8</v>
+      </c>
+      <c r="G2" s="1">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2012</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B4" si="0">D3+F3</f>
+        <v>18.5</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C4" si="1">E3+G3</f>
+        <v>22.4</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F3" s="1">
+        <v>13.3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2017</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>19.100000000000001</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>22.9</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>14.6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>